<commit_message>
Updated Testing Specs and progress
</commit_message>
<xml_diff>
--- a/Research Design/Research Questions and Data Design.xlsx
+++ b/Research Design/Research Questions and Data Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bschuster\Documents\hivergent_analytics\Research Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D713998-CB53-4958-B599-F8F307A34460}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC30347-AA68-4948-8ABE-B1B3A810A31F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="1" xr2:uid="{6DCF36A5-39DC-4EB8-9703-B142A14C83BE}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>What percentage of cryptoassets were being traded across other blockchains such as ripple?</t>
   </si>
@@ -175,15 +175,6 @@
     <t>administrative</t>
   </si>
   <si>
-    <t>Organization Type Must be one of the following</t>
-  </si>
-  <si>
-    <t>ico/token</t>
-  </si>
-  <si>
-    <t>non_fungible_token</t>
-  </si>
-  <si>
     <t>US fee must be to two decimal places</t>
   </si>
   <si>
@@ -233,6 +224,9 @@
   </si>
   <si>
     <t>name_registrar</t>
+  </si>
+  <si>
+    <t>uncategorized</t>
   </si>
 </sst>
 </file>
@@ -918,10 +912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC490C6-9297-4236-8B80-94073C960BD2}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -951,15 +945,15 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -980,6 +974,9 @@
       <c r="D8" t="s">
         <v>44</v>
       </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -988,7 +985,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -997,71 +994,55 @@
         <v>43</v>
       </c>
       <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>64</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" t="s">
-        <v>60</v>
+      <c r="A14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>